<commit_message>
Modified and added ? in Company Gatha file
</commit_message>
<xml_diff>
--- a/interviewprep/Company Gatha.xlsx
+++ b/interviewprep/Company Gatha.xlsx
@@ -336,10 +336,10 @@
     <t xml:space="preserve">public void sum(List&lt;Integer&gt;) and public void sum(List&lt;Double&gt;) will program compile and if so what is output </t>
   </si>
   <si>
-    <t>Are Collection checked at runtime or compile time</t>
-  </si>
-  <si>
     <t>How to avoid referential integrity (many to one or one to many) in hibernate to avoid parent dependency if it gets deleted then implementation on child</t>
+  </si>
+  <si>
+    <t>Are Collection checked at runtime or compile time?</t>
   </si>
 </sst>
 </file>
@@ -861,7 +861,7 @@
   <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E79" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2160,7 +2160,7 @@
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
@@ -2342,7 +2342,7 @@
       <c r="E97" s="14"/>
       <c r="F97" s="14"/>
       <c r="G97" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>

</xml_diff>